<commit_message>
Revised everything to reduce supply requirement by a factor of 10
Did this to keep the cost in line with just hauling LS supplies,
otherwise it was too unbalanced.
</commit_message>
<xml_diff>
--- a/MKS_Worksheet.xlsx
+++ b/MKS_Worksheet.xlsx
@@ -575,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:X87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50:X50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,7 +608,7 @@
     <col min="25" max="16384" width="11.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>54</v>
       </c>
@@ -625,7 +625,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="4" spans="2:24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>53</v>
       </c>
@@ -693,402 +693,501 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" ref="A7:A12" si="0">MAX(C7:CY7)</f>
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="1">
-        <v>-1</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="O7" s="1">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+      <c r="E7">
+        <v>-1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
-      <c r="J9" s="1">
-        <v>-20</v>
-      </c>
-    </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>-1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="1">
-        <v>-1</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+      <c r="D11">
+        <v>-1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="1">
-        <v>-1</v>
-      </c>
-      <c r="F12" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G12" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I12" s="1">
+      <c r="D12">
+        <v>-1</v>
+      </c>
+      <c r="F12">
+        <v>-1</v>
+      </c>
+      <c r="G12">
+        <v>-1</v>
+      </c>
+      <c r="I12">
         <v>-5</v>
       </c>
-      <c r="J12" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
+      <c r="J12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" ref="A14:A20" si="1">MAX(C14:CY14)</f>
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+    <row r="15" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="1">
-        <v>1</v>
-      </c>
-      <c r="F15" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G15" s="1">
-        <v>1</v>
-      </c>
-      <c r="I15" s="1">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>-1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="1">
-        <v>-1</v>
-      </c>
-      <c r="E16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
+      <c r="D16">
+        <v>-1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
         <v>31</v>
       </c>
-      <c r="O17" s="1">
-        <v>20</v>
-      </c>
-      <c r="P17" s="1">
-        <v>-10</v>
-      </c>
-      <c r="Q17" s="1">
-        <v>-10</v>
-      </c>
-      <c r="X17" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+      <c r="O17">
+        <v>2</v>
+      </c>
+      <c r="P17">
+        <v>-1</v>
+      </c>
+      <c r="Q17">
+        <v>-1</v>
+      </c>
+      <c r="X17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
         <v>32</v>
       </c>
-      <c r="M18" s="1">
-        <v>20</v>
-      </c>
-      <c r="Q18" s="1">
-        <v>-10</v>
-      </c>
-      <c r="R18" s="1">
-        <v>-10</v>
-      </c>
-      <c r="X18" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+      <c r="M18">
+        <v>2</v>
+      </c>
+      <c r="Q18">
+        <v>-1</v>
+      </c>
+      <c r="R18">
+        <v>-1</v>
+      </c>
+      <c r="X18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
         <v>33</v>
       </c>
-      <c r="N19" s="1">
-        <v>20</v>
-      </c>
-      <c r="P19" s="1">
-        <v>-10</v>
-      </c>
-      <c r="R19" s="1">
-        <v>-10</v>
-      </c>
-      <c r="X19" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
+      <c r="N19">
+        <v>2</v>
+      </c>
+      <c r="P19">
+        <v>-1</v>
+      </c>
+      <c r="R19">
+        <v>-1</v>
+      </c>
+      <c r="X19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
         <v>34</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
+    <row r="21" spans="1:24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f>MAX(C22:CY22)</f>
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
+    <row r="23" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f>MAX(C23:CY23)</f>
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
         <v>36</v>
       </c>
-      <c r="L23" s="1">
-        <v>-10</v>
-      </c>
-      <c r="P23" s="1">
-        <v>20</v>
-      </c>
-      <c r="T23" s="1">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
+      <c r="L23">
+        <v>-1</v>
+      </c>
+      <c r="P23">
+        <v>2</v>
+      </c>
+      <c r="T23">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f>MAX(C24:CY24)</f>
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
         <v>37</v>
       </c>
-      <c r="R24" s="1">
-        <v>20</v>
-      </c>
-      <c r="S24" s="1">
-        <v>-10</v>
-      </c>
-      <c r="T24" s="1">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
+      <c r="R24">
+        <v>2</v>
+      </c>
+      <c r="S24">
+        <v>-1</v>
+      </c>
+      <c r="T24">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f>MAX(C25:CY25)</f>
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
         <v>38</v>
       </c>
-      <c r="L25" s="1">
-        <v>-10</v>
-      </c>
-      <c r="Q25" s="1">
-        <v>20</v>
-      </c>
-      <c r="S25" s="1">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
+      <c r="L25">
+        <v>-1</v>
+      </c>
+      <c r="Q25">
+        <v>2</v>
+      </c>
+      <c r="S25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" ref="A27:A32" si="2">MAX(C27:CY27)</f>
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
+    <row r="28" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
         <v>40</v>
       </c>
-      <c r="L28" s="1">
-        <v>20</v>
-      </c>
-      <c r="U28" s="1">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="29" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
+      <c r="L28">
+        <v>2</v>
+      </c>
+      <c r="U28">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
         <v>41</v>
       </c>
-      <c r="K29" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
+      <c r="K29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
         <v>42</v>
       </c>
-      <c r="S30" s="1">
-        <v>20</v>
-      </c>
-      <c r="U30" s="1">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
+      <c r="S30">
+        <v>2</v>
+      </c>
+      <c r="U30">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
         <v>43</v>
       </c>
-      <c r="T31" s="1">
-        <v>20</v>
-      </c>
-      <c r="U31" s="1">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="32" spans="2:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T31">
+        <v>2</v>
+      </c>
+      <c r="U31">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
       <c r="B32" t="s">
         <v>44</v>
       </c>
       <c r="E32">
-        <v>-1</v>
+        <v>-0.1</v>
       </c>
       <c r="F32">
-        <v>-1</v>
+        <v>-0.1</v>
       </c>
       <c r="G32">
-        <v>-1</v>
+        <v>-0.1</v>
       </c>
       <c r="H32">
-        <v>-1</v>
+        <v>-0.1</v>
       </c>
       <c r="I32">
-        <v>-1</v>
+        <v>-0.1</v>
       </c>
       <c r="J32">
-        <v>-1</v>
+        <v>-0.1</v>
       </c>
       <c r="K32">
-        <v>-1</v>
+        <v>-0.1</v>
       </c>
       <c r="L32">
-        <v>-1</v>
+        <v>-0.1</v>
       </c>
       <c r="M32">
-        <v>-1</v>
+        <v>-0.1</v>
       </c>
       <c r="N32">
-        <v>-1</v>
+        <v>-0.1</v>
       </c>
       <c r="O32">
-        <v>-1</v>
+        <v>-0.1</v>
       </c>
       <c r="P32">
-        <v>-1</v>
+        <v>-0.1</v>
       </c>
       <c r="Q32">
-        <v>-1</v>
+        <v>-0.1</v>
       </c>
       <c r="R32">
-        <v>-1</v>
+        <v>-0.1</v>
       </c>
       <c r="S32">
-        <v>-1</v>
+        <v>-0.1</v>
       </c>
       <c r="T32">
-        <v>-1</v>
+        <v>-0.1</v>
       </c>
       <c r="U32">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="2:24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>45</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="F33">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="G33">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="I33">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="J33">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="K33">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="L33">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M33">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="N33">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="O33">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="P33">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="Q33">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="R33">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="S33">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="T33">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="X33">
-        <v>-15</v>
-      </c>
-    </row>
-    <row r="34" spans="2:24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="2:24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="2:24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f>MAX(C36:CY36)</f>
+        <v>-20</v>
+      </c>
       <c r="B36" t="s">
         <v>47</v>
       </c>
@@ -1096,10 +1195,14 @@
         <v>-20</v>
       </c>
       <c r="N36">
-        <v>-25</v>
-      </c>
-    </row>
-    <row r="37" spans="2:24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f>MAX(C37:CY37)</f>
+        <v>-20</v>
+      </c>
       <c r="B37" t="s">
         <v>48</v>
       </c>
@@ -1107,10 +1210,14 @@
         <v>-20</v>
       </c>
       <c r="M37">
-        <v>-25</v>
-      </c>
-    </row>
-    <row r="38" spans="2:24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f>MAX(C38:CY38)</f>
+        <v>-5</v>
+      </c>
       <c r="B38" t="s">
         <v>49</v>
       </c>
@@ -1124,7 +1231,11 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="39" spans="2:24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f>MAX(C39:CY39)</f>
+        <v>25</v>
+      </c>
       <c r="B39" t="s">
         <v>50</v>
       </c>
@@ -1180,9 +1291,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="2:24" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="2:24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="2:24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
         <v>55</v>
       </c>
@@ -1198,7 +1309,7 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="2:24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
         <v>57</v>
       </c>
@@ -1214,8 +1325,8 @@
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
     </row>
-    <row r="45" spans="2:24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="2:24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>51</v>
       </c>
@@ -1283,7 +1394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>52</v>
       </c>
@@ -1306,7 +1417,7 @@
         <v>0</v>
       </c>
       <c r="J47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K47">
         <v>0</v>
@@ -1339,7 +1450,7 @@
         <v>1</v>
       </c>
       <c r="U47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V47">
         <v>0</v>
@@ -1351,7 +1462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>56</v>
       </c>
@@ -1380,7 +1491,7 @@
         <v>0</v>
       </c>
       <c r="L48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="M48">
         <v>0</v>
@@ -1392,19 +1503,19 @@
         <v>0</v>
       </c>
       <c r="P48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Q48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="S48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="T48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="U48">
         <v>1</v>
@@ -1416,23 +1527,23 @@
         <v>0</v>
       </c>
       <c r="X48">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:24" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="50" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="5"/>
       <c r="D50" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E50" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F50" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G50" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H50" s="2">
         <v>1</v>
@@ -1447,7 +1558,7 @@
         <v>0</v>
       </c>
       <c r="L50" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M50" s="2">
         <v>0</v>
@@ -1459,22 +1570,22 @@
         <v>0</v>
       </c>
       <c r="P50" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q50" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R50" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S50" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T50" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U50" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V50" s="2">
         <v>0</v>
@@ -1560,559 +1671,559 @@
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
-        <f t="shared" ref="A55:A60" si="0">SUM(C55:CY55)</f>
+        <f t="shared" ref="A55:A60" si="3">SUM(C55:CY55)</f>
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D55" s="1">
-        <f t="shared" ref="D55:X55" si="1">D7*D50</f>
+        <f t="shared" ref="D55:X55" si="4">D7*D50</f>
         <v>0</v>
       </c>
       <c r="E55" s="1">
-        <f t="shared" si="1"/>
-        <v>-6</v>
+        <f t="shared" si="4"/>
+        <v>-10</v>
       </c>
       <c r="F55" s="1">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f t="shared" si="4"/>
+        <v>10</v>
       </c>
       <c r="G55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="R55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="V55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="W55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="X55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
-        <f t="shared" si="0"/>
-        <v>-6</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D56" s="1">
-        <f t="shared" ref="D56:X56" si="2">D8*D50</f>
-        <v>0</v>
+        <f t="shared" ref="D56:X56" si="5">D8*D50</f>
+        <v>10</v>
       </c>
       <c r="E56" s="1">
-        <f t="shared" si="2"/>
-        <v>-6</v>
+        <f t="shared" si="5"/>
+        <v>-10</v>
       </c>
       <c r="F56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="S56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
-        <f t="shared" si="0"/>
-        <v>-8</v>
+        <f t="shared" si="3"/>
+        <v>-5</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D57" s="1">
-        <f t="shared" ref="D57:X57" si="3">D9*D50</f>
-        <v>0</v>
+        <f t="shared" ref="D57:X57" si="6">D9*D50</f>
+        <v>10</v>
       </c>
       <c r="E57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F57" s="1">
-        <f t="shared" si="3"/>
-        <v>6</v>
+        <f t="shared" si="6"/>
+        <v>10</v>
       </c>
       <c r="G57" s="1">
-        <f t="shared" si="3"/>
-        <v>6</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="H57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J57" s="1">
-        <f t="shared" si="3"/>
-        <v>-20</v>
+        <f t="shared" si="6"/>
+        <v>-25</v>
       </c>
       <c r="K57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="W57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="X57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D58" s="1">
-        <f t="shared" ref="D58:X58" si="4">D10*D50</f>
-        <v>0</v>
+        <f t="shared" ref="D58:X58" si="7">D10*D50</f>
+        <v>10</v>
       </c>
       <c r="E58" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F58" s="1">
-        <f t="shared" si="4"/>
-        <v>-6</v>
+        <f t="shared" si="7"/>
+        <v>-10</v>
       </c>
       <c r="G58" s="1">
-        <f t="shared" si="4"/>
-        <v>6</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
       <c r="H58" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I58" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J58" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K58" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L58" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M58" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N58" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O58" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P58" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q58" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R58" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="S58" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T58" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U58" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V58" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W58" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="X58" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D59" s="1">
-        <f t="shared" ref="D59:X59" si="5">D11*D50</f>
-        <v>0</v>
+        <f t="shared" ref="D59:X59" si="8">D11*D50</f>
+        <v>-10</v>
       </c>
       <c r="E59" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F59" s="1">
-        <f t="shared" si="5"/>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>10</v>
       </c>
       <c r="G59" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H59" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I59" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J59" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K59" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L59" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M59" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="N59" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O59" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P59" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q59" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="R59" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="S59" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="T59" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U59" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V59" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W59" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X59" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D60" s="1">
-        <f t="shared" ref="D60:X60" si="6">D12*D50</f>
-        <v>0</v>
+        <f t="shared" ref="D60:X60" si="9">D12*D50</f>
+        <v>-10</v>
       </c>
       <c r="E60" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F60" s="1">
-        <f t="shared" si="6"/>
-        <v>-6</v>
+        <f t="shared" si="9"/>
+        <v>-10</v>
       </c>
       <c r="G60" s="1">
-        <f t="shared" si="6"/>
-        <v>-6</v>
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
       <c r="H60" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I60" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J60" s="1">
-        <f t="shared" si="6"/>
-        <v>20</v>
+        <f t="shared" si="9"/>
+        <v>25</v>
       </c>
       <c r="K60" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="L60" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M60" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N60" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O60" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="P60" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Q60" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="R60" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="S60" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="T60" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U60" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="V60" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="W60" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X60" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2121,652 +2232,652 @@
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
-        <f t="shared" ref="A62:A68" si="7">SUM(C62:CY62)</f>
+        <f t="shared" ref="A62:A68" si="10">SUM(C62:CY62)</f>
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D62" s="1">
-        <f t="shared" ref="D62:X62" si="8">D14*D50</f>
+        <f t="shared" ref="D62:X62" si="11">D14*D50</f>
         <v>0</v>
       </c>
       <c r="E62" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F62" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="G62" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="H62" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="I62" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="J62" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K62" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L62" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="M62" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N62" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="O62" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P62" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q62" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="R62" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S62" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="T62" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U62" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="V62" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W62" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="X62" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D63" s="1">
-        <f t="shared" ref="D63:X63" si="9">D15*D50</f>
+        <f t="shared" ref="D63:X63" si="12">D15*D50</f>
         <v>0</v>
       </c>
       <c r="E63" s="1">
-        <f t="shared" si="9"/>
-        <v>6</v>
+        <f t="shared" si="12"/>
+        <v>10</v>
       </c>
       <c r="F63" s="1">
-        <f t="shared" si="9"/>
-        <v>-6</v>
+        <f t="shared" si="12"/>
+        <v>-10</v>
       </c>
       <c r="G63" s="1">
-        <f t="shared" si="9"/>
-        <v>6</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
       </c>
       <c r="H63" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I63" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="J63" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K63" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="L63" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M63" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="N63" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O63" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P63" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q63" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="R63" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S63" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="T63" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="U63" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="V63" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W63" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X63" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D64" s="1">
-        <f t="shared" ref="D64:X64" si="10">D16*D50</f>
-        <v>0</v>
+        <f t="shared" ref="D64:X64" si="13">D16*D50</f>
+        <v>-10</v>
       </c>
       <c r="E64" s="1">
-        <f t="shared" si="10"/>
-        <v>6</v>
+        <f t="shared" si="13"/>
+        <v>10</v>
       </c>
       <c r="F64" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G64" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H64" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I64" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="J64" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K64" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L64" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M64" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="N64" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="O64" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P64" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Q64" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R64" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="S64" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="T64" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U64" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="V64" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="W64" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="X64" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65" s="6">
-        <f t="shared" si="7"/>
-        <v>5</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D65" s="1">
-        <f t="shared" ref="D65:X65" si="11">D17*D50</f>
+        <f t="shared" ref="D65:X65" si="14">D17*D50</f>
         <v>0</v>
       </c>
       <c r="E65" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="F65" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G65" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H65" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I65" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J65" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K65" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="L65" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M65" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N65" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O65" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="P65" s="1">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>-1</v>
       </c>
       <c r="Q65" s="1">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>-1</v>
       </c>
       <c r="R65" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S65" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="T65" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="U65" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="V65" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="W65" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X65" s="1">
-        <f t="shared" si="11"/>
-        <v>5</v>
+        <f t="shared" si="14"/>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
-        <f t="shared" si="7"/>
-        <v>5</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D66" s="1">
-        <f t="shared" ref="D66:X66" si="12">D18*D50</f>
+        <f t="shared" ref="D66:X66" si="15">D18*D50</f>
         <v>0</v>
       </c>
       <c r="E66" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="F66" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="G66" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="H66" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I66" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="J66" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="K66" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L66" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="M66" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N66" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="O66" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="P66" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="Q66" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>-1</v>
       </c>
       <c r="R66" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>-1</v>
       </c>
       <c r="S66" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T66" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="U66" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="V66" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="W66" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="X66" s="1">
-        <f t="shared" si="12"/>
-        <v>5</v>
+        <f t="shared" si="15"/>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
-        <f t="shared" si="7"/>
-        <v>5</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D67" s="1">
-        <f t="shared" ref="D67:X67" si="13">D19*D50</f>
+        <f t="shared" ref="D67:X67" si="16">D19*D50</f>
         <v>0</v>
       </c>
       <c r="E67" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="F67" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="G67" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H67" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="I67" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="J67" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="K67" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="L67" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="M67" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="N67" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O67" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P67" s="1">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="16"/>
+        <v>-1</v>
       </c>
       <c r="Q67" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="R67" s="1">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="16"/>
+        <v>-1</v>
       </c>
       <c r="S67" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="T67" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U67" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="V67" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="W67" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="X67" s="1">
-        <f t="shared" si="13"/>
-        <v>5</v>
+        <f t="shared" si="16"/>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D68" s="1">
-        <f t="shared" ref="D68:X68" si="14">D20*D50</f>
+        <f t="shared" ref="D68:X68" si="17">D20*D50</f>
         <v>0</v>
       </c>
       <c r="E68" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="F68" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="G68" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="H68" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I68" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="J68" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="K68" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L68" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="M68" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="N68" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="O68" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="P68" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="Q68" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R68" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="S68" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="T68" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="U68" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="V68" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="W68" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="X68" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -2782,87 +2893,87 @@
         <v>35</v>
       </c>
       <c r="D70" s="1">
-        <f t="shared" ref="D70:X70" si="15">D22*D50</f>
+        <f t="shared" ref="D70:X70" si="18">D22*D50</f>
         <v>0</v>
       </c>
       <c r="E70" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="F70" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="G70" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H70" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="I70" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="J70" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K70" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L70" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="M70" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="N70" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="O70" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P70" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Q70" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="R70" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="S70" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="T70" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="U70" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="V70" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="W70" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="X70" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -2875,87 +2986,87 @@
         <v>36</v>
       </c>
       <c r="D71" s="1">
-        <f t="shared" ref="D71:X71" si="16">D23*D50</f>
+        <f t="shared" ref="D71:X71" si="19">D23*D50</f>
         <v>0</v>
       </c>
       <c r="E71" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="F71" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="G71" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="H71" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="I71" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="J71" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="K71" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L71" s="1">
-        <f t="shared" si="16"/>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>-1</v>
       </c>
       <c r="M71" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="N71" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="O71" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="P71" s="1">
-        <f t="shared" si="16"/>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>2</v>
       </c>
       <c r="Q71" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="R71" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="S71" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="T71" s="1">
-        <f t="shared" si="16"/>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>-1</v>
       </c>
       <c r="U71" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="V71" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="W71" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="X71" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -2968,87 +3079,87 @@
         <v>37</v>
       </c>
       <c r="D72" s="1">
-        <f t="shared" ref="D72:X72" si="17">D24*D50</f>
+        <f t="shared" ref="D72:X72" si="20">D24*D50</f>
         <v>0</v>
       </c>
       <c r="E72" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="F72" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="G72" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H72" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="I72" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="J72" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="K72" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="L72" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="M72" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N72" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="O72" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="P72" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="Q72" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="R72" s="1">
-        <f t="shared" si="17"/>
-        <v>0</v>
+        <f t="shared" si="20"/>
+        <v>2</v>
       </c>
       <c r="S72" s="1">
-        <f t="shared" si="17"/>
-        <v>0</v>
+        <f t="shared" si="20"/>
+        <v>-1</v>
       </c>
       <c r="T72" s="1">
-        <f t="shared" si="17"/>
-        <v>0</v>
+        <f t="shared" si="20"/>
+        <v>-1</v>
       </c>
       <c r="U72" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="V72" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="W72" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="X72" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -3061,87 +3172,87 @@
         <v>38</v>
       </c>
       <c r="D73" s="1">
-        <f t="shared" ref="D73:X73" si="18">D25*D50</f>
+        <f t="shared" ref="D73:X73" si="21">D25*D50</f>
         <v>0</v>
       </c>
       <c r="E73" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="F73" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="G73" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="H73" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="I73" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="J73" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="K73" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="L73" s="1">
-        <f t="shared" si="18"/>
-        <v>0</v>
+        <f t="shared" si="21"/>
+        <v>-1</v>
       </c>
       <c r="M73" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="N73" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="O73" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="P73" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="Q73" s="1">
-        <f t="shared" si="18"/>
-        <v>0</v>
+        <f t="shared" si="21"/>
+        <v>2</v>
       </c>
       <c r="R73" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="S73" s="1">
-        <f t="shared" si="18"/>
-        <v>0</v>
+        <f t="shared" si="21"/>
+        <v>-1</v>
       </c>
       <c r="T73" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="U73" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="V73" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="W73" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="X73" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -3150,566 +3261,566 @@
     </row>
     <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
-        <f t="shared" ref="A75:A81" si="19">SUM(C75:CY75)</f>
+        <f t="shared" ref="A75:A81" si="22">SUM(C75:CY75)</f>
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D75" s="1">
-        <f t="shared" ref="D75:X75" si="20">D27*D50</f>
+        <f t="shared" ref="D75:X75" si="23">D27*D50</f>
         <v>0</v>
       </c>
       <c r="E75" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="F75" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="G75" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="H75" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="I75" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="J75" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="K75" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L75" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="M75" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="N75" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="O75" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="P75" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="Q75" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="R75" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="S75" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="T75" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="U75" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="V75" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="W75" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="X75" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A76" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D76" s="1">
-        <f t="shared" ref="D76:X76" si="21">D28*D50</f>
+        <f t="shared" ref="D76:X76" si="24">D28*D50</f>
         <v>0</v>
       </c>
       <c r="E76" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="F76" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="G76" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="H76" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="I76" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="J76" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="K76" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="L76" s="1">
-        <f t="shared" si="21"/>
-        <v>0</v>
+        <f t="shared" si="24"/>
+        <v>2</v>
       </c>
       <c r="M76" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="N76" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="O76" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="P76" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Q76" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="R76" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="S76" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="T76" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="U76" s="1">
-        <f t="shared" si="21"/>
-        <v>0</v>
+        <f t="shared" si="24"/>
+        <v>-2</v>
       </c>
       <c r="V76" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="W76" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="X76" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A77" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D77" s="1">
-        <f t="shared" ref="D77:X77" si="22">D29*D50</f>
+        <f t="shared" ref="D77:X77" si="25">D29*D50</f>
         <v>0</v>
       </c>
       <c r="E77" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="F77" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="G77" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="H77" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="I77" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="J77" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K77" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="L77" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="M77" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="N77" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="O77" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="P77" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="Q77" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="R77" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="S77" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="T77" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="U77" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="V77" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W77" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="X77" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A78" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D78" s="1">
-        <f t="shared" ref="D78:X78" si="23">D30*D50</f>
+        <f t="shared" ref="D78:X78" si="26">D30*D50</f>
         <v>0</v>
       </c>
       <c r="E78" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="F78" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="G78" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="H78" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="I78" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="J78" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="K78" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="L78" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="M78" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="N78" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O78" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="P78" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="Q78" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="R78" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="S78" s="1">
-        <f t="shared" si="23"/>
-        <v>0</v>
+        <f t="shared" si="26"/>
+        <v>2</v>
       </c>
       <c r="T78" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="U78" s="1">
-        <f t="shared" si="23"/>
-        <v>0</v>
+        <f t="shared" si="26"/>
+        <v>-2</v>
       </c>
       <c r="V78" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="W78" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="X78" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A79" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D79" s="1">
-        <f t="shared" ref="D79:X79" si="24">D31*D50</f>
+        <f t="shared" ref="D79:X79" si="27">D31*D50</f>
         <v>0</v>
       </c>
       <c r="E79" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="F79" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="G79" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="H79" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="I79" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="J79" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="K79" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="L79" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="M79" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="N79" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="O79" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="P79" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="Q79" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="R79" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="S79" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="T79" s="1">
-        <f t="shared" si="24"/>
-        <v>0</v>
+        <f t="shared" si="27"/>
+        <v>2</v>
       </c>
       <c r="U79" s="1">
-        <f t="shared" si="24"/>
-        <v>0</v>
+        <f t="shared" si="27"/>
+        <v>-2</v>
       </c>
       <c r="V79" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="W79" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="X79" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A80" s="6">
-        <f t="shared" si="19"/>
-        <v>-20</v>
+        <f t="shared" si="22"/>
+        <v>3.1999999999999993</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D80" s="1">
-        <f t="shared" ref="D80:X80" si="25">D32*D50</f>
+        <f t="shared" ref="D80:X80" si="28">D32*D50</f>
         <v>0</v>
       </c>
       <c r="E80" s="1">
-        <f t="shared" si="25"/>
-        <v>-6</v>
+        <f t="shared" si="28"/>
+        <v>-1</v>
       </c>
       <c r="F80" s="1">
-        <f t="shared" si="25"/>
-        <v>-6</v>
+        <f t="shared" si="28"/>
+        <v>-1</v>
       </c>
       <c r="G80" s="1">
-        <f t="shared" si="25"/>
-        <v>-6</v>
+        <f t="shared" si="28"/>
+        <v>0</v>
       </c>
       <c r="H80" s="1">
-        <f t="shared" si="25"/>
-        <v>-1</v>
+        <f t="shared" si="28"/>
+        <v>-0.1</v>
       </c>
       <c r="I80" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="J80" s="1">
-        <f t="shared" si="25"/>
-        <v>-1</v>
+        <f t="shared" si="28"/>
+        <v>-0.1</v>
       </c>
       <c r="K80" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="L80" s="1">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>-0.1</v>
       </c>
       <c r="M80" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="N80" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="O80" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="P80" s="1">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>-0.1</v>
       </c>
       <c r="Q80" s="1">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>-0.1</v>
       </c>
       <c r="R80" s="1">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>-0.1</v>
       </c>
       <c r="S80" s="1">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>-0.1</v>
       </c>
       <c r="T80" s="1">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>-0.1</v>
       </c>
       <c r="U80" s="1">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>6</v>
       </c>
       <c r="V80" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="W80" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="X80" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A81" s="6">
-        <f t="shared" si="19"/>
-        <v>5</v>
+        <f t="shared" si="22"/>
+        <v>-3.1999999999999993</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>45</v>
@@ -3719,84 +3830,84 @@
         <v>0</v>
       </c>
       <c r="E81" s="1">
-        <f t="shared" ref="E81:X81" si="26">E33*E50</f>
-        <v>6</v>
+        <f t="shared" ref="E81:X81" si="29">E33*E50</f>
+        <v>1</v>
       </c>
       <c r="F81" s="1">
-        <f t="shared" si="26"/>
-        <v>6</v>
+        <f t="shared" si="29"/>
+        <v>1</v>
       </c>
       <c r="G81" s="1">
-        <f t="shared" si="26"/>
-        <v>6</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="H81" s="1">
-        <f t="shared" si="26"/>
-        <v>1</v>
+        <f t="shared" si="29"/>
+        <v>0.1</v>
       </c>
       <c r="I81" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="J81" s="1">
-        <f t="shared" si="26"/>
-        <v>1</v>
+        <f t="shared" si="29"/>
+        <v>0.1</v>
       </c>
       <c r="K81" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="L81" s="1">
-        <f t="shared" si="26"/>
-        <v>0</v>
+        <f t="shared" si="29"/>
+        <v>0.1</v>
       </c>
       <c r="M81" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="N81" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="O81" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="P81" s="1">
-        <f t="shared" si="26"/>
-        <v>0</v>
+        <f t="shared" si="29"/>
+        <v>0.1</v>
       </c>
       <c r="Q81" s="1">
-        <f t="shared" si="26"/>
-        <v>0</v>
+        <f t="shared" si="29"/>
+        <v>0.1</v>
       </c>
       <c r="R81" s="1">
-        <f t="shared" si="26"/>
-        <v>0</v>
+        <f t="shared" si="29"/>
+        <v>0.1</v>
       </c>
       <c r="S81" s="1">
-        <f t="shared" si="26"/>
-        <v>0</v>
+        <f t="shared" si="29"/>
+        <v>0.1</v>
       </c>
       <c r="T81" s="1">
-        <f t="shared" si="26"/>
-        <v>0</v>
+        <f t="shared" si="29"/>
+        <v>0.1</v>
       </c>
       <c r="U81" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="V81" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="W81" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="X81" s="1">
-        <f t="shared" si="26"/>
-        <v>-15</v>
+        <f t="shared" si="29"/>
+        <v>-6</v>
       </c>
     </row>
     <row r="82" spans="1:24" x14ac:dyDescent="0.25">
@@ -3815,71 +3926,71 @@
         <v>0</v>
       </c>
       <c r="E83" s="1">
-        <f t="shared" ref="E83:U83" si="27">E35*E50</f>
+        <f t="shared" ref="E83:U83" si="30">E35*E50</f>
         <v>0</v>
       </c>
       <c r="F83" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="G83" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="H83" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="I83" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="J83" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="K83" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="L83" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="M83" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="N83" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="O83" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="P83" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="Q83" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="R83" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="S83" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="T83" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="U83" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="V83" s="1">
@@ -3908,71 +4019,71 @@
         <v>0</v>
       </c>
       <c r="E84" s="1">
-        <f t="shared" ref="E84:U84" si="28">E36*E50</f>
+        <f t="shared" ref="E84:U84" si="31">E36*E50</f>
         <v>0</v>
       </c>
       <c r="F84" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="G84" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="H84" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="I84" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="J84" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="K84" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="L84" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="M84" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="N84" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="O84" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="P84" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="Q84" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="R84" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="S84" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="T84" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="U84" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="V84" s="1">
@@ -4001,71 +4112,71 @@
         <v>0</v>
       </c>
       <c r="E85" s="1">
-        <f t="shared" ref="E85:U85" si="29">E37*E50</f>
+        <f t="shared" ref="E85:U85" si="32">E37*E50</f>
         <v>0</v>
       </c>
       <c r="F85" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="G85" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="H85" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="I85" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="J85" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="K85" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="L85" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="M85" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="N85" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="O85" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="P85" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="Q85" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R85" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="S85" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="T85" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="U85" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="V85" s="1">
@@ -4084,7 +4195,7 @@
     <row r="86" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A86" s="6">
         <f>SUM(C86:CY86)</f>
-        <v>-30</v>
+        <v>0</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>49</v>
@@ -4094,71 +4205,71 @@
         <v>0</v>
       </c>
       <c r="E86" s="1">
-        <f t="shared" ref="E86:U86" si="30">E38*E50</f>
+        <f t="shared" ref="E86:U86" si="33">E38*E50</f>
         <v>0</v>
       </c>
       <c r="F86" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="G86" s="1">
-        <f t="shared" si="30"/>
-        <v>-30</v>
+        <f t="shared" si="33"/>
+        <v>0</v>
       </c>
       <c r="H86" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="I86" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="J86" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="K86" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="L86" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="M86" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="N86" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="O86" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="P86" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="Q86" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="R86" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="S86" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="T86" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="U86" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="V86" s="1">
@@ -4177,7 +4288,7 @@
     <row r="87" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A87" s="6">
         <f>SUM(C87:CY87)</f>
-        <v>6</v>
+        <v>-3</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>50</v>
@@ -4187,72 +4298,72 @@
         <v>0</v>
       </c>
       <c r="E87" s="1">
-        <f t="shared" ref="E87:U87" si="31">E39*E50</f>
-        <v>-6</v>
+        <f t="shared" ref="E87:U87" si="34">E39*E50</f>
+        <v>-10</v>
       </c>
       <c r="F87" s="1">
-        <f t="shared" si="31"/>
-        <v>-6</v>
+        <f t="shared" si="34"/>
+        <v>-10</v>
       </c>
       <c r="G87" s="1">
-        <f t="shared" si="31"/>
-        <v>-6</v>
+        <f t="shared" si="34"/>
+        <v>0</v>
       </c>
       <c r="H87" s="1">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>25</v>
       </c>
       <c r="I87" s="1">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="J87" s="1">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>-1</v>
       </c>
       <c r="K87" s="1">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="L87" s="1">
-        <f t="shared" si="31"/>
-        <v>0</v>
+        <f t="shared" si="34"/>
+        <v>-1</v>
       </c>
       <c r="M87" s="1">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="N87" s="1">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="O87" s="1">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="P87" s="1">
-        <f t="shared" si="31"/>
-        <v>0</v>
+        <f t="shared" si="34"/>
+        <v>-1</v>
       </c>
       <c r="Q87" s="1">
-        <f t="shared" si="31"/>
-        <v>0</v>
+        <f t="shared" si="34"/>
+        <v>-1</v>
       </c>
       <c r="R87" s="1">
-        <f t="shared" si="31"/>
-        <v>0</v>
+        <f t="shared" si="34"/>
+        <v>-1</v>
       </c>
       <c r="S87" s="1">
-        <f t="shared" si="31"/>
-        <v>0</v>
+        <f t="shared" si="34"/>
+        <v>-1</v>
       </c>
       <c r="T87" s="1">
-        <f t="shared" si="31"/>
-        <v>0</v>
+        <f t="shared" si="34"/>
+        <v>-1</v>
       </c>
       <c r="U87" s="1">
-        <f t="shared" si="31"/>
-        <v>0</v>
+        <f t="shared" si="34"/>
+        <v>-1</v>
       </c>
       <c r="V87" s="1">
         <f>V39*V50</f>

</xml_diff>